<commit_message>
Minor changes, tweaks and fixes.
- Quest Reward Is out of order.
- Quest Reward is not formatted properly.
- New Imports.
- Minor tweaks to drop checks.
</commit_message>
<xml_diff>
--- a/resources/data-imports/skills.xlsx
+++ b/resources/data-imports/skills.xlsx
@@ -15,14 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -120,19 +117,6 @@
   </si>
   <si>
     <t>As you move around the map, using directional buttons only (this will not apply to teleporting, setting sail or teleporting to your own kingdom), you will find, as you get higher in level - that the time is reducing. Train this skill by fighting monsters, to do so - click train on the character sheet for this skill and select how much xp you want to sacrifice to train this skill. Special locations with adventures, can have bonuses applied to skill training.</t>
-  </si>
-  <si>
-    <t>Essence of Speed</t>
-  </si>
-  <si>
-    <t>This skill is trained by you fighting monsters. Over time, this skill will give you roughly 20% off the movement timer for movement based actions such as Teleport (including to your kingdom) and Set Sail</t>
-  </si>
-  <si>
-    <t>Disenchanting</t>
-  </si>
-  <si>
-    <t>This skill cannot be trained by fighting, and there is no button in the action section. Instead, when an item drops in chat, you'll have the option to "disenchant" the item. Or when you select items from your inventory, only those with affixes - when you click disenchant - will be destroyed and you will gain both XP and Gold Dust.
-There is a chance for this skill to fail, resulting in no XP and 1 Gold Dust. You can in stead choose to destroy items, which can only be done via the character sheet - which will provide less gold dust (1-25 per enchanted item). Where as this skill will give you between 1-150 Gold Dust.</t>
   </si>
 </sst>
 </file>
@@ -168,12 +152,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,30 +455,29 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="930" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="37" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="38" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="32" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="41" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="39" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="930" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="37" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="38" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="32" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="41" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="39" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="28" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="25" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="25" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="25" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,22 +514,19 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
+      <c r="C2">
+        <v>999</v>
       </c>
       <c r="D2">
-        <v>999</v>
+        <v>0.0</v>
       </c>
       <c r="E2">
         <v>0.0</v>
@@ -564,361 +541,291 @@
         <v>0.0</v>
       </c>
       <c r="I2">
-        <v>0.0</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>999</v>
+      </c>
+      <c r="D3">
+        <v>0.0</v>
+      </c>
+      <c r="E3">
+        <v>0.0</v>
+      </c>
+      <c r="F3">
+        <v>0.0</v>
+      </c>
+      <c r="G3">
+        <v>0.0</v>
+      </c>
+      <c r="H3">
+        <v>0.0</v>
+      </c>
+      <c r="I3">
         <v>1</v>
-      </c>
-      <c r="L2">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>999</v>
-      </c>
-      <c r="E3">
-        <v>0.0</v>
-      </c>
-      <c r="F3">
-        <v>0.0</v>
-      </c>
-      <c r="G3">
-        <v>0.0</v>
-      </c>
-      <c r="H3">
-        <v>0.0</v>
-      </c>
-      <c r="I3">
-        <v>0.0</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>999</v>
+      </c>
+      <c r="D4">
+        <v>0.0</v>
+      </c>
+      <c r="E4">
+        <v>0.0</v>
+      </c>
+      <c r="F4">
+        <v>0.0</v>
+      </c>
+      <c r="G4">
+        <v>0.0</v>
+      </c>
+      <c r="H4">
+        <v>0.0</v>
+      </c>
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="L3">
+      <c r="K4">
         <v>0.001</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="D4">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>400</v>
+      </c>
+      <c r="D5">
+        <v>0.0</v>
+      </c>
+      <c r="E5">
+        <v>0.0</v>
+      </c>
+      <c r="F5">
+        <v>0.0</v>
+      </c>
+      <c r="G5">
+        <v>0.0</v>
+      </c>
+      <c r="H5">
+        <v>0.0</v>
+      </c>
+      <c r="K5">
+        <v>0.0025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>0.0</v>
+      </c>
+      <c r="E6">
+        <v>0.0</v>
+      </c>
+      <c r="F6">
+        <v>0.0</v>
+      </c>
+      <c r="G6">
+        <v>0.0</v>
+      </c>
+      <c r="H6">
+        <v>0.0</v>
+      </c>
+      <c r="K6">
+        <v>0.0025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>400</v>
+      </c>
+      <c r="D7">
+        <v>0.0</v>
+      </c>
+      <c r="E7">
+        <v>0.0</v>
+      </c>
+      <c r="F7">
+        <v>0.0</v>
+      </c>
+      <c r="G7">
+        <v>0.0</v>
+      </c>
+      <c r="H7">
+        <v>0.0</v>
+      </c>
+      <c r="K7">
+        <v>0.0025</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>400</v>
+      </c>
+      <c r="D8">
+        <v>0.0</v>
+      </c>
+      <c r="E8">
+        <v>0.0</v>
+      </c>
+      <c r="F8">
+        <v>0.0</v>
+      </c>
+      <c r="G8">
+        <v>0.0</v>
+      </c>
+      <c r="H8">
+        <v>0.0</v>
+      </c>
+      <c r="K8">
+        <v>0.0025</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
+        <v>400</v>
+      </c>
+      <c r="D9">
+        <v>0.0</v>
+      </c>
+      <c r="E9">
+        <v>0.0</v>
+      </c>
+      <c r="F9">
+        <v>0.0</v>
+      </c>
+      <c r="G9">
+        <v>0.0</v>
+      </c>
+      <c r="H9">
+        <v>0.0</v>
+      </c>
+      <c r="K9">
+        <v>0.0025</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>400</v>
+      </c>
+      <c r="D10">
+        <v>0.0</v>
+      </c>
+      <c r="E10">
+        <v>0.0</v>
+      </c>
+      <c r="F10">
+        <v>0.0</v>
+      </c>
+      <c r="G10">
+        <v>0.0</v>
+      </c>
+      <c r="H10">
+        <v>0.0</v>
+      </c>
+      <c r="K10">
+        <v>0.0025</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11">
         <v>999</v>
       </c>
-      <c r="E4">
-        <v>0.0</v>
-      </c>
-      <c r="F4">
-        <v>0.0</v>
-      </c>
-      <c r="G4">
-        <v>0.0</v>
-      </c>
-      <c r="H4">
-        <v>0.0</v>
-      </c>
-      <c r="I4">
-        <v>0.0</v>
-      </c>
-      <c r="K4">
+      <c r="D11">
+        <v>0.0</v>
+      </c>
+      <c r="G11">
+        <v>0.0002</v>
+      </c>
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="L4">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5">
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>999</v>
+      </c>
+      <c r="H12">
+        <v>0.0002</v>
+      </c>
+      <c r="J12">
         <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>400</v>
-      </c>
-      <c r="E5">
-        <v>0.0</v>
-      </c>
-      <c r="F5">
-        <v>0.0</v>
-      </c>
-      <c r="G5">
-        <v>0.0</v>
-      </c>
-      <c r="H5">
-        <v>0.0</v>
-      </c>
-      <c r="I5">
-        <v>0.0</v>
-      </c>
-      <c r="L5">
-        <v>0.0025</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>400</v>
-      </c>
-      <c r="E6">
-        <v>0.0</v>
-      </c>
-      <c r="F6">
-        <v>0.0</v>
-      </c>
-      <c r="G6">
-        <v>0.0</v>
-      </c>
-      <c r="H6">
-        <v>0.0</v>
-      </c>
-      <c r="I6">
-        <v>0.0</v>
-      </c>
-      <c r="L6">
-        <v>0.0025</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>400</v>
-      </c>
-      <c r="E7">
-        <v>0.0</v>
-      </c>
-      <c r="F7">
-        <v>0.0</v>
-      </c>
-      <c r="G7">
-        <v>0.0</v>
-      </c>
-      <c r="H7">
-        <v>0.0</v>
-      </c>
-      <c r="I7">
-        <v>0.0</v>
-      </c>
-      <c r="L7">
-        <v>0.0025</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8">
-        <v>400</v>
-      </c>
-      <c r="E8">
-        <v>0.0</v>
-      </c>
-      <c r="F8">
-        <v>0.0</v>
-      </c>
-      <c r="G8">
-        <v>0.0</v>
-      </c>
-      <c r="H8">
-        <v>0.0</v>
-      </c>
-      <c r="I8">
-        <v>0.0</v>
-      </c>
-      <c r="L8">
-        <v>0.0025</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9">
-        <v>400</v>
-      </c>
-      <c r="E9">
-        <v>0.0</v>
-      </c>
-      <c r="F9">
-        <v>0.0</v>
-      </c>
-      <c r="G9">
-        <v>0.0</v>
-      </c>
-      <c r="H9">
-        <v>0.0</v>
-      </c>
-      <c r="I9">
-        <v>0.0</v>
-      </c>
-      <c r="L9">
-        <v>0.0025</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10">
-        <v>400</v>
-      </c>
-      <c r="E10">
-        <v>0.0</v>
-      </c>
-      <c r="F10">
-        <v>0.0</v>
-      </c>
-      <c r="G10">
-        <v>0.0</v>
-      </c>
-      <c r="H10">
-        <v>0.0</v>
-      </c>
-      <c r="I10">
-        <v>0.0</v>
-      </c>
-      <c r="L10">
-        <v>0.0025</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11">
-        <v>999</v>
-      </c>
-      <c r="E11">
-        <v>0.0</v>
-      </c>
-      <c r="H11">
-        <v>0.0002</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12">
-        <v>999</v>
-      </c>
-      <c r="I12">
-        <v>0.0002</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13">
-        <v>999</v>
-      </c>
-      <c r="I13">
-        <v>0.0002</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14">
-        <v>999</v>
-      </c>
-      <c r="L14">
-        <v>0.001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started getting imports into place
</commit_message>
<xml_diff>
--- a/resources/data-imports/skills.xlsx
+++ b/resources/data-imports/skills.xlsx
@@ -15,11 +15,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
     <t>description</t>
   </si>
   <si>
@@ -117,6 +120,19 @@
   </si>
   <si>
     <t>As you move around the map, using directional buttons only (this will not apply to teleporting, setting sail or teleporting to your own kingdom), you will find, as you get higher in level - that the time is reducing. Train this skill by fighting monsters, to do so - click train on the character sheet for this skill and select how much xp you want to sacrifice to train this skill. Special locations with adventures, can have bonuses applied to skill training.</t>
+  </si>
+  <si>
+    <t>Alchemy</t>
+  </si>
+  <si>
+    <t>Alchemy is a skill that is used by you crafting new and magical items that can do one of two things: Devastating damage to kingdoms, or give you boons that can stack and last for a set number of hours.</t>
+  </si>
+  <si>
+    <t>Disenchanting</t>
+  </si>
+  <si>
+    <t>This is used by you disenchanting items that either popup in chat as drops or in your inventory by clicking Disenchant All.
+Should you fail to disenchant an item, you'll only get 1 Gold Dust. Should you succeed you can get between 1 and 150 Gold Dust, where as destroying only gets you 1-25 gold dust and no disenchanting experience.</t>
   </si>
 </sst>
 </file>
@@ -152,9 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,29 +474,30 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="930" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="37" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="38" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="32" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="41" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="39" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="25" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="5" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="930" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="37" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="38" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="32" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="41" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="39" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="28" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="11" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="25" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="25" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,20 +534,23 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
         <v>999</v>
       </c>
-      <c r="D2">
-        <v>0.0</v>
-      </c>
       <c r="E2">
         <v>0.0</v>
       </c>
@@ -541,28 +564,31 @@
         <v>0.0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.0</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
         <v>0.001</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
         <v>999</v>
       </c>
-      <c r="D3">
-        <v>0.0</v>
-      </c>
       <c r="E3">
         <v>0.0</v>
       </c>
@@ -576,28 +602,31 @@
         <v>0.0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0.0</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>0.001</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
         <v>999</v>
       </c>
-      <c r="D4">
-        <v>0.0</v>
-      </c>
       <c r="E4">
         <v>0.0</v>
       </c>
@@ -610,26 +639,29 @@
       <c r="H4">
         <v>0.0</v>
       </c>
-      <c r="J4">
-        <v>1</v>
+      <c r="I4">
+        <v>0.0</v>
       </c>
       <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>0.001</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
         <v>400</v>
       </c>
-      <c r="D5">
-        <v>0.0</v>
-      </c>
       <c r="E5">
         <v>0.0</v>
       </c>
@@ -642,23 +674,26 @@
       <c r="H5">
         <v>0.0</v>
       </c>
-      <c r="K5">
+      <c r="I5">
+        <v>0.0</v>
+      </c>
+      <c r="L5">
         <v>0.0025</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
         <v>400</v>
       </c>
-      <c r="D6">
-        <v>0.0</v>
-      </c>
       <c r="E6">
         <v>0.0</v>
       </c>
@@ -671,23 +706,26 @@
       <c r="H6">
         <v>0.0</v>
       </c>
-      <c r="K6">
+      <c r="I6">
+        <v>0.0</v>
+      </c>
+      <c r="L6">
         <v>0.0025</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C7">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
         <v>400</v>
       </c>
-      <c r="D7">
-        <v>0.0</v>
-      </c>
       <c r="E7">
         <v>0.0</v>
       </c>
@@ -700,23 +738,26 @@
       <c r="H7">
         <v>0.0</v>
       </c>
-      <c r="K7">
+      <c r="I7">
+        <v>0.0</v>
+      </c>
+      <c r="L7">
         <v>0.0025</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C8">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
         <v>400</v>
       </c>
-      <c r="D8">
-        <v>0.0</v>
-      </c>
       <c r="E8">
         <v>0.0</v>
       </c>
@@ -729,23 +770,26 @@
       <c r="H8">
         <v>0.0</v>
       </c>
-      <c r="K8">
+      <c r="I8">
+        <v>0.0</v>
+      </c>
+      <c r="L8">
         <v>0.0025</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C9">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9">
         <v>400</v>
       </c>
-      <c r="D9">
-        <v>0.0</v>
-      </c>
       <c r="E9">
         <v>0.0</v>
       </c>
@@ -758,23 +802,26 @@
       <c r="H9">
         <v>0.0</v>
       </c>
-      <c r="K9">
+      <c r="I9">
+        <v>0.0</v>
+      </c>
+      <c r="L9">
         <v>0.0025</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="C10">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
         <v>400</v>
       </c>
-      <c r="D10">
-        <v>0.0</v>
-      </c>
       <c r="E10">
         <v>0.0</v>
       </c>
@@ -787,45 +834,88 @@
       <c r="H10">
         <v>0.0</v>
       </c>
-      <c r="K10">
+      <c r="I10">
+        <v>0.0</v>
+      </c>
+      <c r="L10">
         <v>0.0025</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C11">
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
         <v>999</v>
       </c>
-      <c r="D11">
-        <v>0.0</v>
-      </c>
-      <c r="G11">
+      <c r="E11">
+        <v>0.0</v>
+      </c>
+      <c r="H11">
         <v>0.0002</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="C12">
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12">
         <v>999</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.0002</v>
       </c>
-      <c r="J12">
-        <v>1</v>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13">
+        <v>400</v>
+      </c>
+      <c r="L13">
+        <v>0.0025</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>999</v>
+      </c>
+      <c r="L14">
+        <v>0.001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed all the tests.
- Moved over towards MYSQl for the tests.
- Fixed every test, removed a few.
- Moved the github actions over to MYSQL
</commit_message>
<xml_diff>
--- a/resources/data-imports/skills.xlsx
+++ b/resources/data-imports/skills.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C29A45B-1F41-3F45-980F-C39E112D78BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Game Skills" sheetId="1" r:id="rId4"/>
+    <sheet name="Game Skills" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>name</t>
   </si>
@@ -53,7 +69,7 @@
     <t>skill_bonus_per_level</t>
   </si>
   <si>
-    <t>specifically_assigned</t>
+    <t>game_class_id</t>
   </si>
   <si>
     <t>is_locked</t>
@@ -113,31 +129,87 @@
     <t>A skill used in enchanting items.</t>
   </si>
   <si>
+    <t>Astral Magics</t>
+  </si>
+  <si>
+    <t>Increases spell damage over time. The higher the level the more spell damage your magics will do. This skill is only available to heritics.
+This bonus is only applied to your spell's that do damage. If you have none equipped, no bonus will be applied.</t>
+  </si>
+  <si>
+    <t>Heretic</t>
+  </si>
+  <si>
+    <t>Celestial Prayer</t>
+  </si>
+  <si>
+    <t>As you level this skill over time, your healing spells will increase over time doing more and more healing.
+This bonus is only applied as long as you have one healing spell equipped.</t>
+  </si>
+  <si>
+    <t>Prophet</t>
+  </si>
+  <si>
+    <t>Soldiers Strength</t>
+  </si>
+  <si>
+    <t>This skill is only applied to fighters. Training this skill will increase your attack and defence as long as you have either a shield (for the defence bonus) or a weapon (for the attack bonus) having both will give you both bonuses, have a weapon (and no shield) or dual wielding, will only give you attack bonus.
+Having double shields will only give you the defence bonus. Having double of either will not mean you get double the bonus, you will only receive the skill bonus(es) once for either type.</t>
+  </si>
+  <si>
+    <t>Fighter</t>
+  </si>
+  <si>
+    <t>Shadow Dance</t>
+  </si>
+  <si>
+    <t>This skill is only applied to thieves and requires the thief to be dual wielding weapons to apply it's bonus. While one might assume thieves are only great with daggers and bows, in this world - a thief can duel wield any set of weapons.
+While duel wielding, this skill will increase your damage over time.
+This will also decrease attack time by ~5% at max level.</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>Blood Lust</t>
+  </si>
+  <si>
+    <t>Only applies to vampires. Unlike other class specific skills vampires do not need any specific equipment for these bonuses to apply to their damage and their healing modifiers.</t>
+  </si>
+  <si>
+    <t>Vampire</t>
+  </si>
+  <si>
+    <t>Natures Insight</t>
+  </si>
+  <si>
+    <t>This skill is only used by rangers. Increasing this skill will apply to attack and fight time out (~5% bonus at max level). Similar to thieves with the exception that these bonuses will only apply if you have a bow equipped.</t>
+  </si>
+  <si>
+    <t>Ranger</t>
+  </si>
+  <si>
     <t>Disenchanting</t>
   </si>
   <si>
-    <t>To disenchant items, all you have to do is either click disenchant in the chat or disenchant all in the inventory section of your character sheet. This will give you between 1-150 gold dust per item, with a chance of failure and only 1 gold dust.
-Items can also be destroyed, but this gives you little gold dust for enchanted items and no disenchanting xp.</t>
+    <t>Allows you to click disenchant to destroy items and get gold dust. The higher the level the more successful at getting the gold dust.
+Destroying items only gets you between 1-25 Gold Dust, guaranteed, while disenchanting can get you between 1-150 or 1 (Gold Dust) if you fail to disenchant.
+Gold dust is used for crafting special items with Alchemy and for conjuring celestial entities.</t>
   </si>
   <si>
     <t>Alchemy</t>
   </si>
   <si>
-    <t>Alchemy is a skill that has to be unlocked via doing a quest. Alchemy allows you to create special items that are usable. Either to damage kingdoms or give your self a temporary boost.
-These items can be sold on the market. If its a item you can use on your self it will only last for so long. If its a item you can use on a kingdom, when you go to attack said kingdom, you will see an extra step before selecting your kingdoms to use said items.</t>
+    <t>Alchemy is a skill that is locked behind a quest. Once unlocked you can click Craft/Enchant to then click a new option called: Alchemy.
+Alchemy requires the use of both Gold Dust (you get from disenchanting and destroying) and Shards (you get from killing (you have to be the one that kills) Celestial Entities). Once you have enough you can start crafting items that either give you limited time boons or items that do damage to kingdoms (which you can only use when attacking a kingdom).
+Boons can be used from your inventory. You can use a maximum of ten boon at one time.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -148,31 +220,40 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -462,35 +543,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:N12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="308" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="37" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="38" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="32" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="41" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="39" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="25" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="25" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="417" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -545,22 +623,22 @@
         <v>15</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>999</v>
       </c>
       <c r="E2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -569,13 +647,13 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -586,22 +664,22 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>999</v>
       </c>
       <c r="E3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -610,13 +688,13 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -627,34 +705,34 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>999</v>
       </c>
       <c r="E4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -668,28 +746,28 @@
         <v>400</v>
       </c>
       <c r="E5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -703,28 +781,28 @@
         <v>400</v>
       </c>
       <c r="E6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -738,28 +816,28 @@
         <v>400</v>
       </c>
       <c r="E7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -773,28 +851,28 @@
         <v>400</v>
       </c>
       <c r="E8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -808,28 +886,28 @@
         <v>400</v>
       </c>
       <c r="E9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -843,33 +921,33 @@
         <v>400</v>
       </c>
       <c r="E10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
@@ -877,45 +955,207 @@
       <c r="D11">
         <v>999</v>
       </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
       <c r="L11">
-        <v>0.001</v>
+        <v>1E-3</v>
+      </c>
+      <c r="M11" t="s">
+        <v>34</v>
       </c>
       <c r="N11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>999</v>
+      </c>
+      <c r="F12">
+        <v>1E-3</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1E-3</v>
+      </c>
+      <c r="M12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>999</v>
+      </c>
+      <c r="E13">
+        <v>1E-3</v>
+      </c>
+      <c r="G13">
+        <v>1E-3</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14">
+        <v>999</v>
+      </c>
+      <c r="E14">
+        <v>1E-3</v>
+      </c>
+      <c r="H14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15">
+        <v>999</v>
+      </c>
+      <c r="E15">
+        <v>1E-3</v>
+      </c>
+      <c r="F15">
+        <v>1E-3</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>46</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16">
+        <v>999</v>
+      </c>
+      <c r="E16">
+        <v>1E-3</v>
+      </c>
+      <c r="H16">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17">
+        <v>999</v>
+      </c>
+      <c r="L17">
+        <v>1E-3</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
         <v>4</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12">
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18">
         <v>400</v>
       </c>
-      <c r="L12">
-        <v>0.0025</v>
-      </c>
-      <c r="N12">
+      <c r="L18">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="N18">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added all the new exports. Fixed a few small issues.
</commit_message>
<xml_diff>
--- a/resources/data-imports/skills.xlsx
+++ b/resources/data-imports/skills.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/1.1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C29A45B-1F41-3F45-980F-C39E112D78BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C32B77B-0257-4143-8CBD-6AFEDAD9E457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>name</t>
   </si>
@@ -202,6 +202,18 @@
     <t>Alchemy is a skill that is locked behind a quest. Once unlocked you can click Craft/Enchant to then click a new option called: Alchemy.
 Alchemy requires the use of both Gold Dust (you get from disenchanting and destroying) and Shards (you get from killing (you have to be the one that kills) Celestial Entities). Once you have enough you can start crafting items that either give you limited time boons or items that do damage to kingdoms (which you can only use when attacking a kingdom).
 Boons can be used from your inventory. You can use a maximum of ten boon at one time.</t>
+  </si>
+  <si>
+    <t>Fighters Resilience</t>
+  </si>
+  <si>
+    <t>The attack timer is 10 seconds by default, how ever with this skill, you can shave off - at max level roughly 20% of those 10 seconds, letting you click more. You level this skill via fighting monsters. Click train on the character sheet and assign some xp, the xp you assign is what you will sacrifice from killing monsters. The higher the percentage, the less xp you get towards leveling when fighting monsters.</t>
+  </si>
+  <si>
+    <t>Quick Feet</t>
+  </si>
+  <si>
+    <t>As you move around the map, using directional buttons only (this will not apply to teleporting, setting sail or teleporting to your own kingdom), you will find, as you get higher in level - that the time is reducing. Train this skill by fighting monsters, to do so - click train on the character sheet for this skill and select how much xp you want to sacrifice to train this skill. Special locations with adventures, can have bonuses applied to skill training.</t>
   </si>
 </sst>
 </file>
@@ -544,17 +556,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="417" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="544" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
@@ -955,11 +967,11 @@
       <c r="D11">
         <v>999</v>
       </c>
+      <c r="E11">
+        <v>1E-3</v>
+      </c>
       <c r="K11">
         <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1E-3</v>
       </c>
       <c r="M11" t="s">
         <v>34</v>
@@ -981,14 +993,14 @@
       <c r="D12">
         <v>999</v>
       </c>
+      <c r="E12">
+        <v>1E-3</v>
+      </c>
       <c r="F12">
         <v>1E-3</v>
       </c>
       <c r="K12">
         <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1E-3</v>
       </c>
       <c r="M12" t="s">
         <v>37</v>
@@ -1043,7 +1055,7 @@
         <v>1E-3</v>
       </c>
       <c r="H14">
-        <v>5.0000000000000001E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1101,7 +1113,7 @@
         <v>1E-3</v>
       </c>
       <c r="H16">
-        <v>5.0000000000000001E-3</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1130,7 +1142,7 @@
         <v>1E-3</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -1151,6 +1163,52 @@
       </c>
       <c r="N18">
         <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19">
+        <v>999</v>
+      </c>
+      <c r="H19">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20">
+        <v>999</v>
+      </c>
+      <c r="I20">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated skills, added new migration.
- Voidance (devouring light) is in place for enemies.
- Voidance is not in place for players, but they are effected by the
  monsters abillityto void them.
</commit_message>
<xml_diff>
--- a/resources/data-imports/skills.xlsx
+++ b/resources/data-imports/skills.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
   <si>
     <t>name</t>
   </si>
@@ -197,6 +197,12 @@
     <t>Alchemy is a skill that is locked behind a quest. Once unlocked you can click Craft/Enchant to then click a new option called: Alchemy.
 Alchemy requires the use of both Gold Dust (you get from disenchanting and destroying) and Shards (you get from killing (you have to be the one that kills) Celestial Entities). Once you have enough you can start crafting items that either give you limited time boons or items that do damage to kingdoms (which you can only use when attacking a kingdom).
 Boons can be used from your inventory. You can use a maximum of ten boon at one time.</t>
+  </si>
+  <si>
+    <t>Casting Accuracy</t>
+  </si>
+  <si>
+    <t>When using any spell - that does damage - this skill will be used to see if your spell hits or fails. The higher the better chance you have to hit your enemy with your spell. Your casting accuracy skill bonus is used to avoid your spells from being evaded. Casters will use 5% of their focus mod + this skill bonus, other classes will just use the skill bonus.</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="C20" sqref="C20"/>
@@ -1193,6 +1199,32 @@
         <v>1</v>
       </c>
     </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21">
+        <v>999</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>0.001</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>

<commit_message>
Finished the core attack portion.
- Rebalanced life stealing affixes.
- Rebalanced Attacks and introduced criticality.

We now just have to do cast, cast and attack, attack and cast and
finally defend.
</commit_message>
<xml_diff>
--- a/resources/data-imports/skills.xlsx
+++ b/resources/data-imports/skills.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>name</t>
   </si>
@@ -203,6 +203,12 @@
   </si>
   <si>
     <t>When using any spell - that does damage - this skill will be used to see if your spell hits or fails. The higher the better chance you have to hit your enemy with your spell. Your casting accuracy skill bonus is used to avoid your spells from being evaded. Casters will use 5% of their focus mod + this skill bonus, other classes will just use the skill bonus.</t>
+  </si>
+  <si>
+    <t>Criticality</t>
+  </si>
+  <si>
+    <t>As you level this skill over time the skill bonus will grow to close to 100%. This bonus is used when you attack enemies to determine if you land a critical attack or not. This only applies to spells (healing and damage) and weapons.</t>
   </si>
 </sst>
 </file>
@@ -544,7 +550,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="C20" sqref="C20"/>
@@ -1004,6 +1010,9 @@
       <c r="E13">
         <v>0.001</v>
       </c>
+      <c r="H13">
+        <v>0.001</v>
+      </c>
       <c r="K13">
         <v>1</v>
       </c>
@@ -1222,6 +1231,29 @@
         <v>0.001</v>
       </c>
       <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22">
+        <v>999</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>0.001</v>
+      </c>
+      <c r="N22">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementing Server checks for some actions.
</commit_message>
<xml_diff>
--- a/resources/data-imports/skills.xlsx
+++ b/resources/data-imports/skills.xlsx
@@ -1,21 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adambalan/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB42BFD-9217-C34B-89BC-C46A010EE320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Game Skills" sheetId="1" r:id="rId4"/>
+    <sheet name="Game Skills" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>name</t>
   </si>
@@ -211,23 +228,27 @@
     <t>As you level this skill over time the skill bonus will grow to close to 100%. This bonus is used when you attack enemies to determine if you land a critical attack or not. This only applies to spells (healing and damage) and weapons.</t>
   </si>
   <si>
-    <t>Lust for Gold</t>
+    <t>Kingmanship</t>
   </si>
   <si>
     <t>With this skill, the more gold you have in your kingdoms treasury, the more interest you gain per hour. The calculation is Gold + Gold * (Skill Bonus + Keep level / 100). Kingdoms can hold a total of two billion gold, while characters can hold 2 trillion gold.</t>
+  </si>
+  <si>
+    <t>Hells Anvil</t>
+  </si>
+  <si>
+    <t>This skill only applies to blacksmiths. The more you level this skill the more defence you will get, you can get up to +200% Attack and +300% Defence.</t>
+  </si>
+  <si>
+    <t>Blacksmith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -238,31 +259,40 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -552,35 +582,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:N23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="544" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="37" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="38" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="32" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="41" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="39" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="28" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="25" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="11" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="544" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -659,13 +686,13 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -700,13 +727,13 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -738,13 +765,13 @@
         <v>1</v>
       </c>
       <c r="L4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -773,13 +800,13 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -808,13 +835,13 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -843,13 +870,13 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -878,13 +905,13 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -913,13 +940,13 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -948,13 +975,13 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="N10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -967,8 +994,14 @@
       <c r="D11">
         <v>999</v>
       </c>
+      <c r="E11">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="G11">
+        <v>7.5000000000000002E-4</v>
+      </c>
       <c r="H11">
-        <v>0.0002</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -977,12 +1010,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
@@ -991,7 +1024,7 @@
         <v>999</v>
       </c>
       <c r="I12">
-        <v>0.0002</v>
+        <v>1E-3</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1000,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1014,10 +1047,10 @@
         <v>999</v>
       </c>
       <c r="E13">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="H13">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1029,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1043,10 +1076,10 @@
         <v>999</v>
       </c>
       <c r="E14">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="F14">
-        <v>0.001</v>
+        <v>1.5E-3</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1058,7 +1091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1072,10 +1105,10 @@
         <v>999</v>
       </c>
       <c r="E15">
-        <v>0.001</v>
+        <v>1.5E-3</v>
       </c>
       <c r="G15">
-        <v>0.001</v>
+        <v>1.5E-3</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1087,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1101,10 +1134,10 @@
         <v>999</v>
       </c>
       <c r="E16">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="H16">
-        <v>5.0E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1116,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1130,10 +1163,10 @@
         <v>999</v>
       </c>
       <c r="E17">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="F17">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -1145,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1159,10 +1192,16 @@
         <v>999</v>
       </c>
       <c r="E18">
-        <v>0.001</v>
+        <v>1E-3</v>
+      </c>
+      <c r="F18">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="G18">
+        <v>1.4999999999999999E-4</v>
       </c>
       <c r="H18">
-        <v>4.0E-5</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1174,7 +1213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1188,13 +1227,13 @@
         <v>999</v>
       </c>
       <c r="L19">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1205,16 +1244,16 @@
         <v>57</v>
       </c>
       <c r="D20">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="L20">
-        <v>0.0025</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="N20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -1234,13 +1273,13 @@
         <v>1</v>
       </c>
       <c r="L21">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -1257,13 +1296,13 @@
         <v>1</v>
       </c>
       <c r="L22">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="N22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -1280,24 +1319,47 @@
         <v>1</v>
       </c>
       <c r="L23">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="N23">
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24">
+        <v>999</v>
+      </c>
+      <c r="E24">
+        <v>1E-3</v>
+      </c>
+      <c r="G24">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24" t="s">
+        <v>66</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>